<commit_message>
added all shapes back to ga runs
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/elongated-pentagonal-bipyramid/elongated-pentagonal-bipyramid_AgAu_data.xlsx
+++ b/data/bimetallic_results/elongated-pentagonal-bipyramid/elongated-pentagonal-bipyramid_AgAu_data.xlsx
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.511096860793739</v>
+        <v>-2.511137773464996</v>
       </c>
       <c r="G24">
         <v>-0.03449633277097108</v>
@@ -967,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>-2.527378959413181</v>
+        <v>-2.527877846873314</v>
       </c>
       <c r="G25">
         <v>-0.03811202385042134</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.629999000998837</v>
+        <v>-2.631810456318401</v>
       </c>
       <c r="G32">
         <v>-0.05231538291777205</v>
@@ -1151,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.646590502516207</v>
+        <v>-2.647108277410378</v>
       </c>
       <c r="G33">
         <v>-0.05509207171540531</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.659353414289208</v>
+        <v>-2.659850806241157</v>
       </c>
       <c r="G34">
         <v>-0.05691240899442218</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.674915991011027</v>
+        <v>-2.675001535374064</v>
       </c>
       <c r="G35">
         <v>-0.0566553053829455</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.780438577850539</v>
+        <v>-2.781476462616934</v>
       </c>
       <c r="G43">
         <v>-0.06492512280120177</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.841876994368953</v>
+        <v>-2.842913730655199</v>
       </c>
       <c r="G48">
         <v>-0.06302854589850393</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.853377361732215</v>
+        <v>-2.853478485389885</v>
       </c>
       <c r="G49">
         <v>-0.06203564695893715</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.876649876959829</v>
+        <v>-2.877360869760938</v>
       </c>
       <c r="G51">
         <v>-0.05993257426714627</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.88682416919193</v>
+        <v>-2.88781439157145</v>
       </c>
       <c r="G52">
         <v>-0.05786114305487211</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-2.952132344440312</v>
+        <v>-2.952653573486972</v>
       </c>
       <c r="G58">
         <v>-0.04713116608712353</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-2.97293321957183</v>
+        <v>-2.973489030509954</v>
       </c>
       <c r="G60">
         <v>-0.04213837133954396</v>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-3.00258873935545</v>
+        <v>-3.002844623212828</v>
       </c>
       <c r="G63">
         <v>-0.03460949088871895</v>
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="F78">
-        <v>-2.582477405892838</v>
+        <v>-2.58254105348469</v>
       </c>
       <c r="G78">
         <v>-0.01290266593950218</v>
@@ -2301,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F83">
-        <v>-2.616074601474897</v>
+        <v>-2.616145631885454</v>
       </c>
       <c r="G83">
         <v>-0.02092322171688599</v>
@@ -2600,7 +2600,7 @@
         <v>24</v>
       </c>
       <c r="F96">
-        <v>-2.698779249213122</v>
+        <v>-2.699045093709665</v>
       </c>
       <c r="G96">
         <v>-0.03859746070860925</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.717604860825898</v>
+        <v>-2.717908093441129</v>
       </c>
       <c r="G99">
         <v>-0.0407730729632938</v>
@@ -2784,7 +2784,7 @@
         <v>32</v>
       </c>
       <c r="F104">
-        <v>-2.74682907877122</v>
+        <v>-2.747628652271021</v>
       </c>
       <c r="G104">
         <v>-0.04616850484636603</v>
@@ -2853,7 +2853,7 @@
         <v>35</v>
       </c>
       <c r="F107">
-        <v>-2.765555480868113</v>
+        <v>-2.766528348043666</v>
       </c>
       <c r="G107">
         <v>-0.04997885708381733</v>
@@ -2968,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="F112">
-        <v>-2.793907240188338</v>
+        <v>-2.796062727539491</v>
       </c>
       <c r="G112">
         <v>-0.050478030493321</v>
@@ -3083,7 +3083,7 @@
         <v>45</v>
       </c>
       <c r="F117">
-        <v>-2.823377397667701</v>
+        <v>-2.823400175757177</v>
       </c>
       <c r="G117">
         <v>-0.0562908823777184</v>
@@ -3175,7 +3175,7 @@
         <v>49</v>
       </c>
       <c r="F121">
-        <v>-2.845559162875121</v>
+        <v>-2.845937888455989</v>
       </c>
       <c r="G121">
         <v>-0.05877331039507538</v>
@@ -3244,7 +3244,7 @@
         <v>52</v>
       </c>
       <c r="F124">
-        <v>-2.863304014956172</v>
+        <v>-2.863841851281895</v>
       </c>
       <c r="G124">
         <v>-0.06088631165212877</v>
@@ -3290,7 +3290,7 @@
         <v>54</v>
       </c>
       <c r="F126">
-        <v>-2.872159132949446</v>
+        <v>-2.872887618371046</v>
       </c>
       <c r="G126">
         <v>-0.06063008521175894</v>
@@ -3336,7 +3336,7 @@
         <v>56</v>
       </c>
       <c r="F128">
-        <v>-2.883890970104383</v>
+        <v>-2.88466417950562</v>
       </c>
       <c r="G128">
         <v>-0.06256056987686343</v>
@@ -3359,7 +3359,7 @@
         <v>57</v>
       </c>
       <c r="F129">
-        <v>-2.889463861049427</v>
+        <v>-2.890819701035323</v>
       </c>
       <c r="G129">
         <v>-0.06309756670556421</v>
@@ -3520,7 +3520,7 @@
         <v>64</v>
       </c>
       <c r="F136">
-        <v>-2.926486542031304</v>
+        <v>-2.927651034089087</v>
       </c>
       <c r="G136">
         <v>-0.06320054470983627</v>
@@ -3612,7 +3612,7 @@
         <v>68</v>
       </c>
       <c r="F140">
-        <v>-2.947154831104334</v>
+        <v>-2.947413996512327</v>
       </c>
       <c r="G140">
         <v>-0.06521029770017517</v>
@@ -3750,7 +3750,7 @@
         <v>74</v>
       </c>
       <c r="F146">
-        <v>-2.97842178918242</v>
+        <v>-2.978605796736173</v>
       </c>
       <c r="G146">
         <v>-0.06642998883671369</v>
@@ -3796,7 +3796,7 @@
         <v>76</v>
       </c>
       <c r="F148">
-        <v>-2.987827495640212</v>
+        <v>-2.987921828038639</v>
       </c>
       <c r="G148">
         <v>-0.06315823744911908</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.027049076795723</v>
+        <v>-3.028597556994702</v>
       </c>
       <c r="G156">
         <v>-0.06373741006675449</v>
@@ -4118,7 +4118,7 @@
         <v>90</v>
       </c>
       <c r="F162">
-        <v>-3.055497690266626</v>
+        <v>-3.055764400675039</v>
       </c>
       <c r="G162">
         <v>-0.06294689008341303</v>
@@ -4210,7 +4210,7 @@
         <v>94</v>
       </c>
       <c r="F166">
-        <v>-3.074533173133353</v>
+        <v>-3.074576372322696</v>
       </c>
       <c r="G166">
         <v>-0.06097622948162984</v>
@@ -4279,7 +4279,7 @@
         <v>97</v>
       </c>
       <c r="F169">
-        <v>-3.087626073767444</v>
+        <v>-3.087779183138879</v>
       </c>
       <c r="G169">
         <v>-0.05879315262597495</v>
@@ -4371,7 +4371,7 @@
         <v>101</v>
       </c>
       <c r="F173">
-        <v>-3.105770486938536</v>
+        <v>-3.107108140217961</v>
       </c>
       <c r="G173">
         <v>-0.05619661795255637</v>
@@ -4394,7 +4394,7 @@
         <v>102</v>
       </c>
       <c r="F174">
-        <v>-3.109621873376897</v>
+        <v>-3.110295732402104</v>
       </c>
       <c r="G174">
         <v>-0.05657591410343865</v>
@@ -4417,7 +4417,7 @@
         <v>103</v>
       </c>
       <c r="F175">
-        <v>-3.113957906070075</v>
+        <v>-3.114103262622178</v>
       </c>
       <c r="G175">
         <v>-0.05464416678249029</v>
@@ -4440,7 +4440,7 @@
         <v>104</v>
       </c>
       <c r="F176">
-        <v>-3.118404510010039</v>
+        <v>-3.11906612529775</v>
       </c>
       <c r="G176">
         <v>-0.05535119219801021</v>
@@ -4463,7 +4463,7 @@
         <v>105</v>
       </c>
       <c r="F177">
-        <v>-3.122991052256344</v>
+        <v>-3.123249507272938</v>
       </c>
       <c r="G177">
         <v>-0.05451272035511234</v>
@@ -4532,7 +4532,7 @@
         <v>108</v>
       </c>
       <c r="F180">
-        <v>-3.135509268863138</v>
+        <v>-3.135655186646941</v>
       </c>
       <c r="G180">
         <v>-0.05231237458573335</v>
@@ -4555,7 +4555,7 @@
         <v>109</v>
       </c>
       <c r="F181">
-        <v>-3.139865092071808</v>
+        <v>-3.140881684319909</v>
       </c>
       <c r="G181">
         <v>-0.05110815729102203</v>
@@ -4601,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="F183">
-        <v>-3.148288811725139</v>
+        <v>-3.148742415234459</v>
       </c>
       <c r="G183">
         <v>-0.04894437230727799</v>
@@ -4739,7 +4739,7 @@
         <v>117</v>
       </c>
       <c r="F189">
-        <v>-3.172200110505028</v>
+        <v>-3.173767241974922</v>
       </c>
       <c r="G189">
         <v>-0.04312406070774544</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="F195">
-        <v>-3.196537363429834</v>
+        <v>-3.196960101427006</v>
       </c>
       <c r="G195">
         <v>-0.03557416378238415</v>
@@ -5015,7 +5015,7 @@
         <v>129</v>
       </c>
       <c r="F201">
-        <v>-3.219231865451615</v>
+        <v>-3.219352448747812</v>
       </c>
       <c r="G201">
         <v>-0.02928001078480946</v>
@@ -5038,7 +5038,7 @@
         <v>130</v>
       </c>
       <c r="F202">
-        <v>-3.223389859328152</v>
+        <v>-3.223798553001189</v>
       </c>
       <c r="G202">
         <v>-0.02940329449118079</v>
@@ -5061,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="F203">
-        <v>-3.227337722599358</v>
+        <v>-3.227381386464581</v>
       </c>
       <c r="G203">
         <v>-0.02780662982893739</v>
@@ -5130,7 +5130,7 @@
         <v>134</v>
       </c>
       <c r="F206">
-        <v>-3.23776747350049</v>
+        <v>-3.237840625351412</v>
       </c>
       <c r="G206">
         <v>-0.02268296112119655</v>
@@ -5153,7 +5153,7 @@
         <v>135</v>
       </c>
       <c r="F207">
-        <v>-3.241924004610194</v>
+        <v>-3.242051648432219</v>
       </c>
       <c r="G207">
         <v>-0.02258006850071517</v>
@@ -5222,7 +5222,7 @@
         <v>138</v>
       </c>
       <c r="F210">
-        <v>-3.251942375758687</v>
+        <v>-3.252376787289037</v>
       </c>
       <c r="G210">
         <v>-0.01766865799096431</v>
@@ -5245,7 +5245,7 @@
         <v>139</v>
       </c>
       <c r="F211">
-        <v>-3.255945964937248</v>
+        <v>-3.256090394221077</v>
       </c>
       <c r="G211">
         <v>-0.015959953087192</v>
@@ -5291,7 +5291,7 @@
         <v>141</v>
       </c>
       <c r="F213">
-        <v>-3.261885290265493</v>
+        <v>-3.262510282202167</v>
       </c>
       <c r="G213">
         <v>-0.01226302225547936</v>
@@ -5314,7 +5314,7 @@
         <v>142</v>
       </c>
       <c r="F214">
-        <v>-3.265038201220376</v>
+        <v>-3.265358029304275</v>
       </c>
       <c r="G214">
         <v>-0.01050632354082642</v>
@@ -5567,7 +5567,7 @@
         <v>154</v>
       </c>
       <c r="F225">
-        <v>-3.078805366803566</v>
+        <v>-3.079166431108553</v>
       </c>
       <c r="G225">
         <v>-0.06489045909411528</v>
@@ -5590,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="F226">
-        <v>-3.152462856986095</v>
+        <v>-3.152717086243879</v>
       </c>
       <c r="G226">
         <v>-0.0614763946049619</v>
@@ -5636,7 +5636,7 @@
         <v>247</v>
       </c>
       <c r="F228">
-        <v>-3.287034081079529</v>
+        <v>-3.28728540842361</v>
       </c>
       <c r="G228">
         <v>-0.04108423754776991</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.345714766432807</v>
+        <v>-3.346929097287571</v>
       </c>
       <c r="G229">
         <v>-0.02394448519907111</v>
@@ -5728,7 +5728,7 @@
         <v>56</v>
       </c>
       <c r="F232">
-        <v>-2.794455079300617</v>
+        <v>-2.794489723356777</v>
       </c>
       <c r="G232">
         <v>-0.02557133017608226</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-2.980698635625816</v>
+        <v>-2.980828057267124</v>
       </c>
       <c r="G234">
         <v>-0.05615996382956001</v>
@@ -5866,7 +5866,7 @@
         <v>392</v>
       </c>
       <c r="F238">
-        <v>-3.291058861599091</v>
+        <v>-3.29155619567054</v>
       </c>
       <c r="G238">
         <v>-0.05341448146908667</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.266787407213697</v>
+        <v>-3.267345568786862</v>
       </c>
       <c r="G248">
         <v>-0.05914424075405922</v>
@@ -6303,7 +6303,7 @@
         <v>566</v>
       </c>
       <c r="F257">
-        <v>-3.142202058853327</v>
+        <v>-3.142404511814147</v>
       </c>
       <c r="G257">
         <v>-0.05860433794154263</v>
@@ -6349,7 +6349,7 @@
         <v>849</v>
       </c>
       <c r="F259">
-        <v>-3.301396318520953</v>
+        <v>-3.302006159021204</v>
       </c>
       <c r="G259">
         <v>-0.05847773367816367</v>
@@ -6395,7 +6395,7 @@
         <v>1132</v>
       </c>
       <c r="F261">
-        <v>-3.442861442607177</v>
+        <v>-3.443017254085076</v>
       </c>
       <c r="G261">
         <v>-0.03928450472781986</v>
@@ -6418,7 +6418,7 @@
         <v>1273</v>
       </c>
       <c r="F262">
-        <v>-3.506193720388489</v>
+        <v>-3.506263178935096</v>
       </c>
       <c r="G262">
         <v>-0.02247821198851802</v>
@@ -6579,7 +6579,7 @@
         <v>1028</v>
       </c>
       <c r="F269">
-        <v>-3.248474692552624</v>
+        <v>-3.24855135639198</v>
       </c>
       <c r="G269">
         <v>-0.06068763153889112</v>
@@ -7016,7 +7016,7 @@
         <v>774</v>
       </c>
       <c r="F288">
-        <v>-3.020454185503217</v>
+        <v>-3.020637203982579</v>
       </c>
       <c r="G288">
         <v>-0.04176292599700115</v>
@@ -7131,7 +7131,7 @@
         <v>2709</v>
       </c>
       <c r="F293">
-        <v>-3.439460808189694</v>
+        <v>-3.439930909652832</v>
       </c>
       <c r="G293">
         <v>-0.05026536224583411</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.574932932205309</v>
+        <v>-3.57494679207619</v>
       </c>
       <c r="G295">
         <v>-0.02195919404188035</v>

</xml_diff>